<commit_message>
Add requirements.txt for Flask and openpyxl dependencies
</commit_message>
<xml_diff>
--- a/Kopiko_Habit_Tracker.xlsx
+++ b/Kopiko_Habit_Tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://woodplc-my.sharepoint.com/personal/andrew_loke_woodplc_com1/Documents/04_Code/Tracking_Kopiko/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="11_7BA50B9D9A6C386FE31D5C5556D6C63FAD8C1CFB" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F6E312A4-AF15-4F14-8481-8C896A6D1AC1}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="11_7BA50B9D9A6C386FE31D5C5556D6C63FAD8C1CFB" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1FAAC711-F3FB-4E7E-A754-113BF978C07E}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Year</t>
   </si>
@@ -54,6 +54,9 @@
   </si>
   <si>
     <t>After Food?</t>
+  </si>
+  <si>
+    <t>Timestamp</t>
   </si>
 </sst>
 </file>
@@ -371,10 +374,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -385,7 +388,7 @@
     <col min="7" max="7" width="14.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -406,6 +409,9 @@
       </c>
       <c r="G1" t="s">
         <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>